<commit_message>
Intégration graphisme Daedalus + Quartiers (terminé)
</commit_message>
<xml_diff>
--- a/#AUTRES/Fichiers texte Genius/Classement scènes Unity.xlsx
+++ b/#AUTRES/Fichiers texte Genius/Classement scènes Unity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NOUVEAU\Desktop\Genius\#AUTRES\Fichiers texte Genius\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6246666C-6A00-4721-BC2D-AA2D494304A1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254DB5AB-3AAF-457B-8A7E-86EEB559DFB5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9255" xr2:uid="{CAD78F56-36D4-40C2-A86C-580F30ECBFC0}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" xr2:uid="{CAD78F56-36D4-40C2-A86C-580F30ECBFC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Catégorie</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>Trophées</t>
+  </si>
+  <si>
+    <t>AffaireDroit</t>
   </si>
 </sst>
 </file>
@@ -625,7 +628,7 @@
   <dimension ref="A1:I111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -688,7 +691,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -708,7 +711,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>14</v>
@@ -728,7 +731,7 @@
         <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>15</v>
@@ -748,7 +751,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
@@ -766,7 +769,7 @@
         <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
@@ -784,7 +787,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
@@ -802,7 +805,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
@@ -818,7 +821,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
@@ -832,7 +835,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
@@ -846,7 +849,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
@@ -860,7 +863,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
@@ -874,7 +877,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
@@ -888,7 +891,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
@@ -901,7 +904,9 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
         <v>54</v>

</xml_diff>